<commit_message>
Atualização planilha de orçamento
</commit_message>
<xml_diff>
--- a/PastaDocsAdministrativos/Orcamento.xlsx
+++ b/PastaDocsAdministrativos/Orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logonrmlocal\Downloads\GITExercicio\3SIPG-ExemploGit-2024\PastaDocsAdministrativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E95C242-6CA2-4B9B-AD76-DEC53166B216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8067FCEF-16BE-469E-BDC1-A33C1B0E6D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>PREVISÃO ORÇAMENTÁRIA - PROJETO EXEMPLO</t>
   </si>
   <si>
     <t>Item de gasto</t>
+  </si>
+  <si>
+    <t>Valor Mensal Previsto</t>
   </si>
 </sst>
 </file>
@@ -79,19 +82,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,21 +393,26 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>